<commit_message>
some text added by anand
anand
</commit_message>
<xml_diff>
--- a/SnaaOOH Beta Version-Links.xlsx
+++ b/SnaaOOH Beta Version-Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>http://54.179.76.169/beta/home</t>
   </si>
@@ -193,6 +193,9 @@
 UN:abc@gmail.com PWD:87654321.
 UN:info@gmail.com Pwd:12345678
 UN::velubala17@gmail.co PWD:12345678</t>
+  </si>
+  <si>
+    <t>//this text added by anand</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -861,6 +864,11 @@
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>